<commit_message>
added expand with multiple system versions test
</commit_message>
<xml_diff>
--- a/postman-tests/FHIR Terminology Server API Testing Status C36.xlsx
+++ b/postman-tests/FHIR Terminology Server API Testing Status C36.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryantaustin/Projects/ecqm/cqf-measures-local/postman-tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F34D4CC-C915-1F4D-AA24-02C71E978650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{441198BB-133F-A24E-BF9E-25ED812ACBEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="520" yWindow="2660" windowWidth="34200" windowHeight="17500" xr2:uid="{0D5B6508-2202-490B-81AD-3E791A748B4C}"/>
+    <workbookView xWindow="8420" yWindow="1440" windowWidth="34200" windowHeight="17500" xr2:uid="{0D5B6508-2202-490B-81AD-3E791A748B4C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -148,7 +147,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="243">
   <si>
     <t>Requirement</t>
   </si>
@@ -877,6 +876,12 @@
   </si>
   <si>
     <t>Value Set 6.8: Representation (Publishable) Value Set EffectiveDate uses dateTime</t>
+  </si>
+  <si>
+    <t>Phase II</t>
+  </si>
+  <si>
+    <t>Value Set 12.19: Expand (Multiple System Versions)</t>
   </si>
 </sst>
 </file>
@@ -993,9 +998,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1033,7 +1038,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1139,7 +1144,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1281,7 +1286,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1289,10 +1294,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9B69458-3FFD-47F5-B370-45CE081B01AB}">
-  <dimension ref="A1:K205"/>
+  <dimension ref="A1:K206"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
+      <selection activeCell="A137" sqref="A137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2569,48 +2574,45 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>225</v>
+        <v>242</v>
+      </c>
+      <c r="B137" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>68</v>
-      </c>
-      <c r="B143" t="s">
-        <v>128</v>
-      </c>
-      <c r="C143" t="s">
-        <v>131</v>
+        <v>230</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B144" t="s">
         <v>128</v>
@@ -2621,62 +2623,59 @@
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B145" t="s">
         <v>128</v>
       </c>
       <c r="C145" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>71</v>
+        <v>70</v>
+      </c>
+      <c r="B146" t="s">
+        <v>128</v>
+      </c>
+      <c r="C146" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
         <v>149</v>
       </c>
-      <c r="B147" t="s">
+      <c r="B148" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="148" spans="1:7" ht="48" x14ac:dyDescent="0.2">
-      <c r="A148" t="s">
+    <row r="149" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
         <v>72</v>
       </c>
-      <c r="B148" t="s">
-        <v>128</v>
-      </c>
-      <c r="C148" t="s">
-        <v>129</v>
-      </c>
-      <c r="E148" s="2" t="s">
+      <c r="B149" t="s">
+        <v>128</v>
+      </c>
+      <c r="C149" t="s">
+        <v>129</v>
+      </c>
+      <c r="E149" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="G148" s="2" t="s">
+      <c r="G149" s="2" t="s">
         <v>144</v>
-      </c>
-    </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A149" t="s">
-        <v>73</v>
-      </c>
-      <c r="B149" t="s">
-        <v>128</v>
-      </c>
-      <c r="E149" t="s">
-        <v>133</v>
-      </c>
-      <c r="G149" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B150" t="s">
         <v>128</v>
@@ -2690,82 +2689,88 @@
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B151" t="s">
         <v>128</v>
       </c>
-      <c r="C151" t="s">
-        <v>129</v>
-      </c>
       <c r="E151" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="G151" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B152" t="s">
         <v>128</v>
       </c>
+      <c r="C152" t="s">
+        <v>129</v>
+      </c>
       <c r="E152" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="G152" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B153" t="s">
         <v>128</v>
       </c>
-      <c r="C153" t="s">
-        <v>129</v>
-      </c>
       <c r="E153" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="G153" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B154" t="s">
         <v>128</v>
       </c>
+      <c r="C154" t="s">
+        <v>129</v>
+      </c>
       <c r="E154" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="G154" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>79</v>
+        <v>78</v>
+      </c>
+      <c r="B155" t="s">
+        <v>128</v>
+      </c>
+      <c r="E155" t="s">
+        <v>133</v>
+      </c>
+      <c r="G155" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>80</v>
-      </c>
-      <c r="C156" t="s">
-        <v>186</v>
+        <v>79</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C157" t="s">
         <v>186</v>
@@ -2773,7 +2778,7 @@
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C158" t="s">
         <v>186</v>
@@ -2781,32 +2786,29 @@
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C159" t="s">
         <v>186</v>
-      </c>
-      <c r="E159" t="s">
-        <v>133</v>
-      </c>
-      <c r="G159" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C160" t="s">
         <v>186</v>
+      </c>
+      <c r="E160" t="s">
+        <v>133</v>
+      </c>
+      <c r="G160" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>85</v>
-      </c>
-      <c r="B161" t="s">
-        <v>128</v>
+        <v>84</v>
       </c>
       <c r="C161" t="s">
         <v>186</v>
@@ -2814,7 +2816,7 @@
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B162" t="s">
         <v>128</v>
@@ -2825,7 +2827,10 @@
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>86</v>
+        <v>87</v>
+      </c>
+      <c r="B163" t="s">
+        <v>128</v>
       </c>
       <c r="C163" t="s">
         <v>186</v>
@@ -2833,7 +2838,7 @@
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C164" t="s">
         <v>186</v>
@@ -2841,10 +2846,7 @@
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>89</v>
-      </c>
-      <c r="B165" t="s">
-        <v>128</v>
+        <v>88</v>
       </c>
       <c r="C165" t="s">
         <v>186</v>
@@ -2852,7 +2854,10 @@
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>90</v>
+        <v>89</v>
+      </c>
+      <c r="B166" t="s">
+        <v>128</v>
       </c>
       <c r="C166" t="s">
         <v>186</v>
@@ -2860,7 +2865,7 @@
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C167" t="s">
         <v>186</v>
@@ -2868,10 +2873,7 @@
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>92</v>
-      </c>
-      <c r="B168" t="s">
-        <v>128</v>
+        <v>91</v>
       </c>
       <c r="C168" t="s">
         <v>186</v>
@@ -2879,41 +2881,29 @@
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
+        <v>92</v>
+      </c>
+      <c r="B169" t="s">
+        <v>128</v>
+      </c>
+      <c r="C169" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="170" spans="1:9" ht="112" x14ac:dyDescent="0.2">
-      <c r="A170" t="s">
+    <row r="171" spans="1:9" ht="112" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
         <v>94</v>
       </c>
-      <c r="B170" t="s">
-        <v>128</v>
-      </c>
-      <c r="C170" t="s">
-        <v>129</v>
-      </c>
-      <c r="E170" t="s">
-        <v>136</v>
-      </c>
-      <c r="G170" t="s">
-        <v>136</v>
-      </c>
-      <c r="H170" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="I170" s="2" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A171" t="s">
-        <v>95</v>
-      </c>
       <c r="B171" t="s">
         <v>128</v>
       </c>
       <c r="C171" t="s">
-        <v>186</v>
+        <v>129</v>
       </c>
       <c r="E171" t="s">
         <v>136</v>
@@ -2921,21 +2911,36 @@
       <c r="G171" t="s">
         <v>136</v>
       </c>
+      <c r="H171" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="I171" s="2" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B172" t="s">
         <v>128</v>
       </c>
       <c r="C172" t="s">
         <v>186</v>
+      </c>
+      <c r="E172" t="s">
+        <v>136</v>
+      </c>
+      <c r="G172" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>137</v>
+        <v>96</v>
+      </c>
+      <c r="B173" t="s">
+        <v>128</v>
       </c>
       <c r="C173" t="s">
         <v>186</v>
@@ -2943,15 +2948,15 @@
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>231</v>
+        <v>137</v>
       </c>
       <c r="C174" t="s">
-        <v>129</v>
+        <v>186</v>
       </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C175" t="s">
         <v>129</v>
@@ -2959,15 +2964,15 @@
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>97</v>
+        <v>232</v>
       </c>
       <c r="C176" t="s">
-        <v>186</v>
+        <v>129</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C177" t="s">
         <v>186</v>
@@ -2975,7 +2980,7 @@
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C178" t="s">
         <v>186</v>
@@ -2983,7 +2988,7 @@
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C179" t="s">
         <v>186</v>
@@ -2991,7 +2996,7 @@
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C180" t="s">
         <v>186</v>
@@ -2999,7 +3004,7 @@
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C181" t="s">
         <v>186</v>
@@ -3007,7 +3012,7 @@
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C182" t="s">
         <v>186</v>
@@ -3015,7 +3020,7 @@
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C183" t="s">
         <v>186</v>
@@ -3023,7 +3028,7 @@
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C184" t="s">
         <v>186</v>
@@ -3031,32 +3036,23 @@
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C185" t="s">
-        <v>129</v>
+        <v>186</v>
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>107</v>
-      </c>
-      <c r="B186" t="s">
-        <v>138</v>
+        <v>106</v>
       </c>
       <c r="C186" t="s">
         <v>129</v>
-      </c>
-      <c r="E186" t="s">
-        <v>135</v>
-      </c>
-      <c r="G186" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B187" t="s">
         <v>138</v>
@@ -3073,7 +3069,7 @@
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B188" t="s">
         <v>138</v>
@@ -3090,7 +3086,7 @@
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B189" t="s">
         <v>138</v>
@@ -3107,7 +3103,7 @@
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B190" t="s">
         <v>138</v>
@@ -3124,7 +3120,7 @@
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B191" t="s">
         <v>138</v>
@@ -3141,29 +3137,35 @@
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B192" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="C192" t="s">
         <v>129</v>
+      </c>
+      <c r="E192" t="s">
+        <v>135</v>
+      </c>
+      <c r="G192" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>114</v>
+        <v>113</v>
+      </c>
+      <c r="B193" t="s">
+        <v>128</v>
       </c>
       <c r="C193" t="s">
-        <v>186</v>
+        <v>129</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>115</v>
-      </c>
-      <c r="B194" t="s">
-        <v>138</v>
+        <v>114</v>
       </c>
       <c r="C194" t="s">
         <v>186</v>
@@ -3171,7 +3173,7 @@
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B195" t="s">
         <v>138</v>
@@ -3182,7 +3184,7 @@
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B196" t="s">
         <v>138</v>
@@ -3193,7 +3195,7 @@
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B197" t="s">
         <v>138</v>
@@ -3204,7 +3206,7 @@
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B198" t="s">
         <v>138</v>
@@ -3215,7 +3217,7 @@
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B199" t="s">
         <v>138</v>
@@ -3226,10 +3228,10 @@
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B200" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="C200" t="s">
         <v>186</v>
@@ -3237,7 +3239,10 @@
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>122</v>
+        <v>121</v>
+      </c>
+      <c r="B201" t="s">
+        <v>128</v>
       </c>
       <c r="C201" t="s">
         <v>186</v>
@@ -3245,10 +3250,7 @@
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>123</v>
-      </c>
-      <c r="B202" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C202" t="s">
         <v>186</v>
@@ -3256,7 +3258,7 @@
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B203" t="s">
         <v>128</v>
@@ -3267,7 +3269,7 @@
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B204" t="s">
         <v>128</v>
@@ -3278,12 +3280,23 @@
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
+        <v>125</v>
+      </c>
+      <c r="B205" t="s">
+        <v>128</v>
+      </c>
+      <c r="C205" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A206" t="s">
         <v>126</v>
       </c>
-      <c r="B205" t="s">
-        <v>128</v>
-      </c>
-      <c r="C205" t="s">
+      <c r="B206" t="s">
+        <v>128</v>
+      </c>
+      <c r="C206" t="s">
         <v>129</v>
       </c>
     </row>

</xml_diff>

<commit_message>
testing results from connectathon
</commit_message>
<xml_diff>
--- a/postman-tests/FHIR Terminology Server API Testing Status C36.xlsx
+++ b/postman-tests/FHIR Terminology Server API Testing Status C36.xlsx
@@ -8,12 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryantaustin/Projects/ecqm/cqf-measures-local/postman-tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{441198BB-133F-A24E-BF9E-25ED812ACBEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ABEF330-8240-B24B-B1EE-646879EA0524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8420" yWindow="1440" windowWidth="34200" windowHeight="17500" xr2:uid="{0D5B6508-2202-490B-81AD-3E791A748B4C}"/>
+    <workbookView xWindow="10920" yWindow="1440" windowWidth="24920" windowHeight="17500" xr2:uid="{0D5B6508-2202-490B-81AD-3E791A748B4C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="General Summary" sheetId="2" r:id="rId1"/>
+    <sheet name="VSAC Results" sheetId="3" r:id="rId2"/>
+    <sheet name="Apelon Results" sheetId="4" r:id="rId3"/>
+    <sheet name="Hl7 Results" sheetId="5" r:id="rId4"/>
+    <sheet name="OCL Results" sheetId="6" r:id="rId5"/>
+    <sheet name="Requirements" sheetId="1" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -147,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="258">
   <si>
     <t>Requirement</t>
   </si>
@@ -883,12 +888,57 @@
   <si>
     <t>Value Set 12.19: Expand (Multiple System Versions)</t>
   </si>
+  <si>
+    <t>Server</t>
+  </si>
+  <si>
+    <t>Requests</t>
+  </si>
+  <si>
+    <t>Test-scripts</t>
+  </si>
+  <si>
+    <t>Prerequest-scripts</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Total Assertions</t>
+  </si>
+  <si>
+    <t>Pass %</t>
+  </si>
+  <si>
+    <t>https://uat-cts.nlm.nih.gov/fhir/</t>
+  </si>
+  <si>
+    <t>http://fhir.ext.apelon.com:7080/dtsserverws/fhir/</t>
+  </si>
+  <si>
+    <t>https://fhir.staging.openconceptlab.org/fhir/</t>
+  </si>
+  <si>
+    <t>http://tx.fhir.org/r4</t>
+  </si>
+  <si>
+    <t>Test Title</t>
+  </si>
+  <si>
+    <t>Failures - expected behavior</t>
+  </si>
+  <si>
+    <t>Actual Behavior</t>
+  </si>
+  <si>
+    <t>Timeout</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -951,6 +1001,28 @@
       <name val="Menlo"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -969,10 +1041,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -980,8 +1053,18 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1293,10 +1376,271 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4668FAE5-85DD-6043-ACC5-81D9C0696DC2}">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="H1" s="5"/>
+    </row>
+    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="B2" s="6">
+        <v>113</v>
+      </c>
+      <c r="C2" s="6">
+        <v>225</v>
+      </c>
+      <c r="D2" s="6">
+        <v>115</v>
+      </c>
+      <c r="E2" s="6">
+        <v>93</v>
+      </c>
+      <c r="F2" s="6">
+        <v>692</v>
+      </c>
+      <c r="G2" s="6">
+        <f>INT((F2-E2)/F2*100)</f>
+        <v>86</v>
+      </c>
+      <c r="H2" s="6"/>
+    </row>
+    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="B3" s="6">
+        <v>113</v>
+      </c>
+      <c r="C3" s="6">
+        <v>225</v>
+      </c>
+      <c r="D3" s="6">
+        <v>115</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6" t="e">
+        <f t="shared" ref="G3:G5" si="0">INT((F3-E3)/F3*100)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="B4" s="6">
+        <v>113</v>
+      </c>
+      <c r="C4" s="6">
+        <v>225</v>
+      </c>
+      <c r="D4" s="6">
+        <v>115</v>
+      </c>
+      <c r="E4" s="6">
+        <v>437</v>
+      </c>
+      <c r="F4" s="6">
+        <v>692</v>
+      </c>
+      <c r="G4" s="6">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B5" s="6">
+        <v>113</v>
+      </c>
+      <c r="C5" s="6">
+        <v>225</v>
+      </c>
+      <c r="D5" s="6">
+        <v>115</v>
+      </c>
+      <c r="E5" s="6">
+        <v>337</v>
+      </c>
+      <c r="F5" s="6">
+        <v>692</v>
+      </c>
+      <c r="G5" s="6">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="H5" s="6"/>
+    </row>
+    <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{5F4899FA-D7E8-7348-94EC-C0828E638888}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{9D922D75-2C11-BD42-9DA2-2C415559989A}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{8FEEE1EA-B723-6445-BF3D-996B2F441DEA}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{80BE874C-3A3D-B745-887E-00035AAB03B0}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75784DF6-A0E2-BD4F-B6C3-4DF6225DD89B}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="38" customWidth="1"/>
+    <col min="2" max="2" width="29.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="8" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>256</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAE83535-C134-5547-B1AE-53DE8A8CD38D}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" s="8" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>256</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC82A74B-7E58-C747-A0BA-E511C05B5AE0}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" s="8" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>256</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4EBFDE9-7534-A148-BD0A-7F5C2430A8CC}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" s="8" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>256</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9B69458-3FFD-47F5-B370-45CE081B01AB}">
   <dimension ref="A1:K206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
+    <sheetView topLeftCell="A44" workbookViewId="0">
       <selection activeCell="A137" sqref="A137"/>
     </sheetView>
   </sheetViews>

</xml_diff>